<commit_message>
Update Box and Lid Excel File
</commit_message>
<xml_diff>
--- a/Documents/Box and Lid Combination/Box and Lid Combination Data Sheet.xlsx
+++ b/Documents/Box and Lid Combination/Box and Lid Combination Data Sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://technionchina-my.sharepoint.com/personal/zeng12875_gtiit_edu_cn/Documents/学习/大三下/Project_in_Design_for_Manufacturing/Project-in-Design-2024/Documents/Box and Lid Combination/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GTIIT\Semester 6_Spring 2024\Design project\Box and Lid Combination\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{0D599F48-BC2D-403B-BC5F-D8E0E1A3D841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{29E1F637-2CF0-EA4C-B84F-555B9A74CA84}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2097BED9-DFDA-4B78-BCA5-FACF83EE3A92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="31560" windowHeight="17980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="33">
   <si>
     <t>Motor mass [kg]</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -143,13 +143,48 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Total Mass [kg]</t>
-  </si>
-  <si>
-    <t>Weight [N]</t>
-  </si>
-  <si>
     <t>Density [kg/mm^3]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shaft coupling [kg]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>density of pipe beam [kg/mm^3]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>volume of beam [mm^3]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>beam pipe</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>box length</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>aphla deg</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>d mm</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ws mm</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>w mm</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>safety factor</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -160,7 +195,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -172,7 +207,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -211,7 +246,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -299,11 +334,52 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -311,6 +387,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -329,30 +411,12 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -364,39 +428,143 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -742,43 +910,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:M40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="132" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.5" style="2" customWidth="1"/>
-    <col min="2" max="5" width="15.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="30.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.83203125" style="1" customWidth="1"/>
-    <col min="8" max="16" width="15.83203125" customWidth="1"/>
+    <col min="1" max="1" width="15.5546875" style="2" customWidth="1"/>
+    <col min="2" max="5" width="15.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="30.5546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.77734375" style="1" customWidth="1"/>
+    <col min="8" max="16" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="6">
+      <c r="G1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="29"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="8">
         <v>9.81</v>
       </c>
       <c r="B2" s="1">
@@ -793,93 +969,93 @@
       <c r="E2" s="1">
         <v>0.36399999999999999</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="1">
         <f>E4+D4+C4</f>
         <v>5.3194430700000002</v>
       </c>
-      <c r="G2" s="26" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="27"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="6"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="29"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
+      <c r="G2" s="2">
+        <v>1.8846999999999999E-2</v>
+      </c>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="21"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="8"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="21"/>
+    </row>
+    <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="16">
         <f>$A$2*B2</f>
         <v>12.50775</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="16">
         <f t="shared" ref="C4:E4" si="0">$A$2*C2</f>
         <v>0.88434207000000009</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="16">
         <f t="shared" si="0"/>
         <v>0.86426100000000006</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="16">
         <f t="shared" si="0"/>
         <v>3.57084</v>
       </c>
-      <c r="F4" s="7"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="28"/>
-      <c r="L4" s="29"/>
-    </row>
-    <row r="5" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="21"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
-      <c r="L5" s="29"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="23" t="s">
+      <c r="F4" s="16"/>
+      <c r="G4" s="4">
+        <f>$A$2*G2</f>
+        <v>0.18488906999999999</v>
+      </c>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="22"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="18"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="52" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="H5" s="53"/>
+      <c r="I5" s="53"/>
+      <c r="J5" s="53"/>
+      <c r="K5" s="53"/>
+      <c r="L5" s="54"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="28"/>
-      <c r="K6" s="28"/>
-      <c r="L6" s="29"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
+      <c r="F6" s="9"/>
+      <c r="G6" s="55"/>
+      <c r="H6" s="56"/>
+      <c r="I6" s="56"/>
+      <c r="J6" s="56"/>
+      <c r="K6" s="56"/>
+      <c r="L6" s="57"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>7</v>
@@ -890,198 +1066,198 @@
       <c r="E7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="7"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="28"/>
-      <c r="K7" s="28"/>
-      <c r="L7" s="29"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="9">
-        <v>1326400.577</v>
-      </c>
-      <c r="B8" s="10">
+      <c r="F7" s="9"/>
+      <c r="G7" s="55"/>
+      <c r="H7" s="56"/>
+      <c r="I7" s="56"/>
+      <c r="J7" s="56"/>
+      <c r="K7" s="56"/>
+      <c r="L7" s="57"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="31">
+        <v>949430</v>
+      </c>
+      <c r="B8" s="25">
         <v>7.8499999999999994E-6</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="23">
         <f t="shared" ref="C8:C13" si="1">$A$8*B8</f>
-        <v>10.41224452945</v>
-      </c>
-      <c r="D8" s="11">
-        <v>2.3253E-4</v>
-      </c>
-      <c r="E8" s="11">
-        <v>1.7885</v>
-      </c>
-      <c r="F8" s="12" t="s">
+        <v>7.453025499999999</v>
+      </c>
+      <c r="D8" s="23">
+        <v>1.8736E-4</v>
+      </c>
+      <c r="E8" s="23">
+        <v>1.7786999999999999</v>
+      </c>
+      <c r="F8" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
-      <c r="I8" s="28"/>
-      <c r="J8" s="28"/>
-      <c r="K8" s="28"/>
-      <c r="L8" s="29"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="13"/>
-      <c r="B9" s="14">
+      <c r="G8" s="55"/>
+      <c r="H8" s="56"/>
+      <c r="I8" s="56"/>
+      <c r="J8" s="56"/>
+      <c r="K8" s="56"/>
+      <c r="L8" s="57"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="12"/>
+      <c r="B9" s="26">
         <v>2.7700000000000002E-6</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="27">
         <f t="shared" si="1"/>
-        <v>3.6741295982900004</v>
+        <v>2.6299211000000002</v>
       </c>
       <c r="D9" s="1">
-        <v>6.5653E-4</v>
+        <v>5.3541999999999999E-4</v>
       </c>
       <c r="E9" s="1">
-        <v>1.7857000000000001</v>
-      </c>
-      <c r="F9" s="7" t="s">
+        <v>1.7766</v>
+      </c>
+      <c r="F9" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="28"/>
-      <c r="K9" s="28"/>
-      <c r="L9" s="29"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="6"/>
-      <c r="B10" s="14">
+      <c r="G9" s="55"/>
+      <c r="H9" s="56"/>
+      <c r="I9" s="56"/>
+      <c r="J9" s="56"/>
+      <c r="K9" s="56"/>
+      <c r="L9" s="57"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="8"/>
+      <c r="B10" s="26">
         <v>8.3000000000000002E-6</v>
       </c>
       <c r="C10" s="1">
         <f t="shared" si="1"/>
-        <v>11.009124789100001</v>
-      </c>
-      <c r="F10" s="7" t="s">
+        <v>7.8802690000000002</v>
+      </c>
+      <c r="F10" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="28"/>
-      <c r="K10" s="28"/>
-      <c r="L10" s="29"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="6"/>
-      <c r="B11" s="14">
+      <c r="G10" s="55"/>
+      <c r="H10" s="56"/>
+      <c r="I10" s="56"/>
+      <c r="J10" s="56"/>
+      <c r="K10" s="56"/>
+      <c r="L10" s="57"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="8"/>
+      <c r="B11" s="26">
         <v>4.6199999999999998E-6</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="27">
         <f t="shared" si="1"/>
-        <v>6.1279706657400004</v>
+        <v>4.3863665999999997</v>
       </c>
       <c r="D11" s="1">
-        <v>4.9176999999999999E-4</v>
+        <v>4.0146000000000002E-4</v>
       </c>
       <c r="E11" s="1">
-        <v>1.7825</v>
-      </c>
-      <c r="F11" s="7" t="s">
+        <v>1.7738</v>
+      </c>
+      <c r="F11" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="28"/>
-      <c r="K11" s="28"/>
-      <c r="L11" s="29"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" s="6"/>
-      <c r="B12" s="14">
+      <c r="G11" s="55"/>
+      <c r="H11" s="56"/>
+      <c r="I11" s="56"/>
+      <c r="J11" s="56"/>
+      <c r="K11" s="56"/>
+      <c r="L11" s="57"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="8"/>
+      <c r="B12" s="26">
         <v>7.7500000000000003E-6</v>
       </c>
       <c r="C12" s="1">
         <f t="shared" si="1"/>
-        <v>10.279604471750002</v>
-      </c>
-      <c r="F12" s="7" t="s">
+        <v>7.3580825000000001</v>
+      </c>
+      <c r="F12" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28"/>
-      <c r="I12" s="28"/>
-      <c r="J12" s="28"/>
-      <c r="K12" s="28"/>
-      <c r="L12" s="29"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="6"/>
-      <c r="B13" s="14">
+      <c r="G12" s="55"/>
+      <c r="H12" s="56"/>
+      <c r="I12" s="56"/>
+      <c r="J12" s="56"/>
+      <c r="K12" s="56"/>
+      <c r="L12" s="57"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="8"/>
+      <c r="B13" s="26">
         <v>1.7999999999999999E-6</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C13" s="27">
         <f t="shared" si="1"/>
-        <v>2.3875210386000001</v>
-      </c>
-      <c r="D13" s="16">
-        <v>1.0443E-3</v>
-      </c>
-      <c r="E13" s="16">
-        <v>1.7836000000000001</v>
-      </c>
-      <c r="F13" s="17" t="s">
+        <v>1.708974</v>
+      </c>
+      <c r="D13" s="24">
+        <v>8.5260999999999996E-4</v>
+      </c>
+      <c r="E13" s="24">
+        <v>1.7747999999999999</v>
+      </c>
+      <c r="F13" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G13" s="28"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="28"/>
-      <c r="K13" s="28"/>
-      <c r="L13" s="29"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="6"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="28"/>
-      <c r="K14" s="28"/>
-      <c r="L14" s="29"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="6"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="28"/>
-      <c r="L15" s="29"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="6"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="28"/>
-      <c r="K16" s="28"/>
-      <c r="L16" s="29"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="8" t="s">
+      <c r="G13" s="55"/>
+      <c r="H13" s="56"/>
+      <c r="I13" s="56"/>
+      <c r="J13" s="56"/>
+      <c r="K13" s="56"/>
+      <c r="L13" s="57"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="8"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="55"/>
+      <c r="H14" s="56"/>
+      <c r="I14" s="56"/>
+      <c r="J14" s="56"/>
+      <c r="K14" s="56"/>
+      <c r="L14" s="57"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="8"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="55"/>
+      <c r="H15" s="56"/>
+      <c r="I15" s="56"/>
+      <c r="J15" s="56"/>
+      <c r="K15" s="56"/>
+      <c r="L15" s="57"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="8"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="55"/>
+      <c r="H16" s="56"/>
+      <c r="I16" s="56"/>
+      <c r="J16" s="56"/>
+      <c r="K16" s="56"/>
+      <c r="L16" s="57"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="F17" s="7"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="28"/>
-      <c r="J17" s="28"/>
-      <c r="K17" s="28"/>
-      <c r="L17" s="29"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
+      <c r="F17" s="9"/>
+      <c r="G17" s="55"/>
+      <c r="H17" s="56"/>
+      <c r="I17" s="56"/>
+      <c r="J17" s="56"/>
+      <c r="K17" s="56"/>
+      <c r="L17" s="57"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" s="8" t="s">
         <v>12</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1096,19 +1272,19 @@
       <c r="E18" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="7"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="28"/>
-      <c r="K18" s="28"/>
-      <c r="L18" s="29"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" s="13">
+      <c r="F18" s="9"/>
+      <c r="G18" s="55"/>
+      <c r="H18" s="56"/>
+      <c r="I18" s="56"/>
+      <c r="J18" s="56"/>
+      <c r="K18" s="56"/>
+      <c r="L18" s="57"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="12">
         <v>2047100</v>
       </c>
-      <c r="B19" s="14">
+      <c r="B19" s="26">
         <v>7.8499999999999994E-6</v>
       </c>
       <c r="C19" s="1">
@@ -1116,140 +1292,430 @@
         <v>16.069734999999998</v>
       </c>
       <c r="D19" s="1">
-        <v>1.4690999999999999E-4</v>
+        <v>1.3852999999999999E-4</v>
       </c>
       <c r="E19" s="1">
         <v>1.5971</v>
       </c>
-      <c r="F19" s="12" t="s">
+      <c r="F19" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G19" s="28"/>
-      <c r="H19" s="28"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="28"/>
-      <c r="K19" s="28"/>
-      <c r="L19" s="29"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" s="6"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="28"/>
-      <c r="J20" s="28"/>
-      <c r="K20" s="28"/>
-      <c r="L20" s="29"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" s="6"/>
-      <c r="B21" s="24" t="s">
+      <c r="G19" s="55"/>
+      <c r="H19" s="56"/>
+      <c r="I19" s="56"/>
+      <c r="J19" s="56"/>
+      <c r="K19" s="56"/>
+      <c r="L19" s="57"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" s="8"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="55"/>
+      <c r="H20" s="56"/>
+      <c r="I20" s="56"/>
+      <c r="J20" s="56"/>
+      <c r="K20" s="56"/>
+      <c r="L20" s="57"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" s="8"/>
+      <c r="B21" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24" t="s">
+      <c r="C21" s="51"/>
+      <c r="D21" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="24"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="28"/>
-      <c r="I21" s="28"/>
-      <c r="J21" s="28"/>
-      <c r="K21" s="28"/>
-      <c r="L21" s="29"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" s="6"/>
-      <c r="B22" s="25">
+      <c r="E21" s="51"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="55"/>
+      <c r="H21" s="56"/>
+      <c r="I21" s="56"/>
+      <c r="J21" s="56"/>
+      <c r="K21" s="56"/>
+      <c r="L21" s="57"/>
+    </row>
+    <row r="22" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="14"/>
+      <c r="B22" s="61">
         <f>(C19-C13)/C19</f>
-        <v>0.85142747913391237</v>
-      </c>
-      <c r="C22" s="25"/>
-      <c r="D22" s="25">
+        <v>0.89365263335083001</v>
+      </c>
+      <c r="C22" s="61"/>
+      <c r="D22" s="61">
         <f>D13-D19</f>
-        <v>8.9738999999999997E-4</v>
-      </c>
-      <c r="E22" s="25"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28"/>
-      <c r="I22" s="28"/>
-      <c r="J22" s="28"/>
-      <c r="K22" s="28"/>
-      <c r="L22" s="29"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" s="6"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="28"/>
-      <c r="I23" s="28"/>
-      <c r="J23" s="28"/>
-      <c r="K23" s="28"/>
-      <c r="L23" s="29"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" s="6"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="28"/>
-      <c r="H24" s="28"/>
-      <c r="I24" s="28"/>
-      <c r="J24" s="28"/>
-      <c r="K24" s="28"/>
-      <c r="L24" s="29"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25" s="6"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="28"/>
-      <c r="H25" s="28"/>
-      <c r="I25" s="28"/>
-      <c r="J25" s="28"/>
-      <c r="K25" s="28"/>
-      <c r="L25" s="29"/>
-    </row>
-    <row r="26" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="18"/>
-      <c r="B26" s="20"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="30"/>
-      <c r="H26" s="30"/>
-      <c r="I26" s="30"/>
-      <c r="J26" s="30"/>
-      <c r="K26" s="30"/>
-      <c r="L26" s="31"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
+        <v>7.1407999999999997E-4</v>
+      </c>
+      <c r="E22" s="61"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="58"/>
+      <c r="H22" s="59"/>
+      <c r="I22" s="59"/>
+      <c r="J22" s="59"/>
+      <c r="K22" s="59"/>
+      <c r="L22" s="60"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B23" s="23"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="20"/>
+      <c r="L23" s="20"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="51"/>
+      <c r="D24" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" s="51"/>
+      <c r="G24" s="51"/>
+      <c r="H24" s="51"/>
+      <c r="I24" s="51"/>
+      <c r="J24" s="51"/>
+      <c r="K24" s="51"/>
+      <c r="L24" s="51"/>
+      <c r="M24" s="51"/>
+    </row>
+    <row r="25" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="2">
+        <v>2965705.784</v>
+      </c>
+      <c r="B25" s="51">
+        <f>0.0000009357</f>
+        <v>9.3569999999999999E-7</v>
+      </c>
+      <c r="C25" s="51"/>
+      <c r="F25" s="51"/>
+      <c r="G25" s="51"/>
+      <c r="H25" s="51"/>
+      <c r="I25" s="51"/>
+      <c r="J25" s="51"/>
+      <c r="K25" s="51"/>
+      <c r="L25" s="51"/>
+      <c r="M25" s="51"/>
+    </row>
+    <row r="26" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="30">
+        <f>A25*B25</f>
+        <v>2.7750109020888001</v>
+      </c>
+      <c r="F26" s="62"/>
+      <c r="G26" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="H26" s="40"/>
+      <c r="I26" s="40"/>
+      <c r="J26" s="40"/>
+      <c r="K26" s="40"/>
+      <c r="L26" s="33"/>
+      <c r="M26" s="63"/>
+    </row>
+    <row r="27" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F27" s="62"/>
+      <c r="G27" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="H27" s="40" t="s">
         <v>22</v>
       </c>
+      <c r="I27" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="J27" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="K27" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="L27" s="33"/>
+      <c r="M27" s="63"/>
+    </row>
+    <row r="28" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F28" s="62"/>
+      <c r="G28" s="37">
+        <v>949430</v>
+      </c>
+      <c r="H28" s="41">
+        <v>7.8499999999999994E-6</v>
+      </c>
+      <c r="I28" s="44">
+        <f t="shared" ref="I28:I33" si="2">$A$8*H28</f>
+        <v>7.453025499999999</v>
+      </c>
+      <c r="J28" s="44">
+        <v>1.8736E-4</v>
+      </c>
+      <c r="K28" s="44">
+        <v>1.7786999999999999</v>
+      </c>
+      <c r="L28" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="M28" s="63"/>
+    </row>
+    <row r="29" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="2">
+        <f>C29+E29*TAN(RADIANS(B29))+2*D29/COS(RADIANS(B29))</f>
+        <v>93.069200243157383</v>
+      </c>
       <c r="B29" s="1">
-        <f>B2+C2*2+D2*2+E2*2+C13</f>
-        <v>4.7470150385999998</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B30" s="1">
-        <f>9.81*B29</f>
-        <v>46.568217528666004</v>
-      </c>
+        <v>22.5</v>
+      </c>
+      <c r="C29" s="1">
+        <v>30</v>
+      </c>
+      <c r="D29" s="1">
+        <v>10</v>
+      </c>
+      <c r="E29" s="1">
+        <v>100</v>
+      </c>
+      <c r="F29" s="62"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="42">
+        <v>2.7700000000000002E-6</v>
+      </c>
+      <c r="I29" s="45">
+        <f t="shared" si="2"/>
+        <v>2.6299211000000002</v>
+      </c>
+      <c r="J29" s="40">
+        <v>5.3541999999999999E-4</v>
+      </c>
+      <c r="K29" s="40">
+        <v>1.7766</v>
+      </c>
+      <c r="L29" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="M29" s="63"/>
+    </row>
+    <row r="30" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E30" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F30" s="62"/>
+      <c r="G30" s="36"/>
+      <c r="H30" s="42">
+        <v>8.3000000000000002E-6</v>
+      </c>
+      <c r="I30" s="40">
+        <f t="shared" si="2"/>
+        <v>7.8802690000000002</v>
+      </c>
+      <c r="J30" s="40"/>
+      <c r="K30" s="40"/>
+      <c r="L30" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="M30" s="63"/>
+    </row>
+    <row r="31" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="2">
+        <f>A29*E31</f>
+        <v>116.33650030394674</v>
+      </c>
+      <c r="E31" s="1">
+        <v>1.25</v>
+      </c>
+      <c r="F31" s="62"/>
+      <c r="G31" s="36"/>
+      <c r="H31" s="42">
+        <v>4.6199999999999998E-6</v>
+      </c>
+      <c r="I31" s="45">
+        <f t="shared" si="2"/>
+        <v>4.3863665999999997</v>
+      </c>
+      <c r="J31" s="40">
+        <v>4.0146000000000002E-4</v>
+      </c>
+      <c r="K31" s="40">
+        <v>1.7738</v>
+      </c>
+      <c r="L31" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="M31" s="63"/>
+    </row>
+    <row r="32" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F32" s="62"/>
+      <c r="G32" s="36"/>
+      <c r="H32" s="42">
+        <v>7.7500000000000003E-6</v>
+      </c>
+      <c r="I32" s="40">
+        <f t="shared" si="2"/>
+        <v>7.3580825000000001</v>
+      </c>
+      <c r="J32" s="40"/>
+      <c r="K32" s="40"/>
+      <c r="L32" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="M32" s="63"/>
+    </row>
+    <row r="33" spans="6:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F33" s="62"/>
+      <c r="G33" s="39"/>
+      <c r="H33" s="43">
+        <v>1.7999999999999999E-6</v>
+      </c>
+      <c r="I33" s="46">
+        <f t="shared" si="2"/>
+        <v>1.708974</v>
+      </c>
+      <c r="J33" s="47">
+        <v>8.5260999999999996E-4</v>
+      </c>
+      <c r="K33" s="47">
+        <v>1.7747999999999999</v>
+      </c>
+      <c r="L33" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="M33" s="63"/>
+    </row>
+    <row r="34" spans="6:13" x14ac:dyDescent="0.3">
+      <c r="F34" s="51"/>
+      <c r="G34" s="51"/>
+      <c r="H34" s="51"/>
+      <c r="I34" s="51"/>
+      <c r="J34" s="51"/>
+      <c r="K34" s="51"/>
+      <c r="L34" s="51"/>
+      <c r="M34" s="51"/>
+    </row>
+    <row r="35" spans="6:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F35" s="51"/>
+      <c r="G35" s="51"/>
+      <c r="H35" s="51"/>
+      <c r="I35" s="51"/>
+      <c r="J35" s="51"/>
+      <c r="K35" s="51"/>
+      <c r="L35" s="51"/>
+      <c r="M35" s="51"/>
+    </row>
+    <row r="36" spans="6:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F36" s="62"/>
+      <c r="G36" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="H36" s="40"/>
+      <c r="I36" s="40"/>
+      <c r="J36" s="40"/>
+      <c r="K36" s="40"/>
+      <c r="L36" s="33"/>
+      <c r="M36" s="63"/>
+    </row>
+    <row r="37" spans="6:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F37" s="62"/>
+      <c r="G37" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="H37" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="I37" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="J37" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="K37" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="L37" s="33"/>
+      <c r="M37" s="63"/>
+    </row>
+    <row r="38" spans="6:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F38" s="62"/>
+      <c r="G38" s="49">
+        <v>2047100</v>
+      </c>
+      <c r="H38" s="43">
+        <v>7.8499999999999994E-6</v>
+      </c>
+      <c r="I38" s="50">
+        <f>$A$19*H38</f>
+        <v>16.069734999999998</v>
+      </c>
+      <c r="J38" s="50">
+        <v>1.3852999999999999E-4</v>
+      </c>
+      <c r="K38" s="50">
+        <v>1.5971</v>
+      </c>
+      <c r="L38" s="48" t="s">
+        <v>11</v>
+      </c>
+      <c r="M38" s="63"/>
+    </row>
+    <row r="39" spans="6:13" x14ac:dyDescent="0.3">
+      <c r="F39" s="51"/>
+      <c r="G39" s="51"/>
+      <c r="H39" s="51"/>
+      <c r="I39" s="51"/>
+      <c r="J39" s="51"/>
+      <c r="K39" s="51"/>
+      <c r="L39" s="51"/>
+      <c r="M39" s="51"/>
+    </row>
+    <row r="40" spans="6:13" x14ac:dyDescent="0.3">
+      <c r="F40" s="51"/>
+      <c r="G40" s="51"/>
+      <c r="H40" s="51"/>
+      <c r="I40" s="51"/>
+      <c r="J40" s="51"/>
+      <c r="K40" s="51"/>
+      <c r="L40" s="51"/>
+      <c r="M40" s="51"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="14">
+    <mergeCell ref="F39:M40"/>
+    <mergeCell ref="F26:F33"/>
+    <mergeCell ref="M26:M33"/>
+    <mergeCell ref="F34:M35"/>
+    <mergeCell ref="F36:F38"/>
+    <mergeCell ref="M36:M38"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="G5:L22"/>
     <mergeCell ref="D21:E21"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B22:C22"/>
-    <mergeCell ref="G2:L26"/>
+    <mergeCell ref="F24:M25"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Box and Lid excel file modification
</commit_message>
<xml_diff>
--- a/Documents/Box and Lid Combination/Box and Lid Combination Data Sheet.xlsx
+++ b/Documents/Box and Lid Combination/Box and Lid Combination Data Sheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GTIIT\Semester 6_Spring 2024\Design project\Box and Lid Combination\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GTIIT\Semester 6_Spring 2024\design_project_github\Project-in-Design-2024\Documents\Box and Lid Combination\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2097BED9-DFDA-4B78-BCA5-FACF83EE3A92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE229DE1-DA22-488E-A542-E0E8288FC7D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
   <si>
     <t>Motor mass [kg]</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -246,7 +246,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -334,52 +334,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -470,63 +429,6 @@
     <xf numFmtId="11" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -560,10 +462,30 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -912,8 +834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1029,26 +951,26 @@
       <c r="D5" s="19"/>
       <c r="E5" s="19"/>
       <c r="F5" s="7"/>
-      <c r="G5" s="52" t="e" vm="1">
+      <c r="G5" s="33" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="H5" s="53"/>
-      <c r="I5" s="53"/>
-      <c r="J5" s="53"/>
-      <c r="K5" s="53"/>
-      <c r="L5" s="54"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="34"/>
+      <c r="L5" s="35"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>19</v>
       </c>
       <c r="F6" s="9"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="56"/>
-      <c r="I6" s="56"/>
-      <c r="J6" s="56"/>
-      <c r="K6" s="56"/>
-      <c r="L6" s="57"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="37"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="38"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
@@ -1067,12 +989,12 @@
         <v>10</v>
       </c>
       <c r="F7" s="9"/>
-      <c r="G7" s="55"/>
-      <c r="H7" s="56"/>
-      <c r="I7" s="56"/>
-      <c r="J7" s="56"/>
-      <c r="K7" s="56"/>
-      <c r="L7" s="57"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="37"/>
+      <c r="L7" s="38"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="31">
@@ -1094,12 +1016,12 @@
       <c r="F8" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="55"/>
-      <c r="H8" s="56"/>
-      <c r="I8" s="56"/>
-      <c r="J8" s="56"/>
-      <c r="K8" s="56"/>
-      <c r="L8" s="57"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37"/>
+      <c r="J8" s="37"/>
+      <c r="K8" s="37"/>
+      <c r="L8" s="38"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="12"/>
@@ -1119,12 +1041,12 @@
       <c r="F9" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="55"/>
-      <c r="H9" s="56"/>
-      <c r="I9" s="56"/>
-      <c r="J9" s="56"/>
-      <c r="K9" s="56"/>
-      <c r="L9" s="57"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="37"/>
+      <c r="J9" s="37"/>
+      <c r="K9" s="37"/>
+      <c r="L9" s="38"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="8"/>
@@ -1138,12 +1060,12 @@
       <c r="F10" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="55"/>
-      <c r="H10" s="56"/>
-      <c r="I10" s="56"/>
-      <c r="J10" s="56"/>
-      <c r="K10" s="56"/>
-      <c r="L10" s="57"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="37"/>
+      <c r="J10" s="37"/>
+      <c r="K10" s="37"/>
+      <c r="L10" s="38"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="8"/>
@@ -1163,12 +1085,12 @@
       <c r="F11" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="55"/>
-      <c r="H11" s="56"/>
-      <c r="I11" s="56"/>
-      <c r="J11" s="56"/>
-      <c r="K11" s="56"/>
-      <c r="L11" s="57"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="37"/>
+      <c r="J11" s="37"/>
+      <c r="K11" s="37"/>
+      <c r="L11" s="38"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="8"/>
@@ -1182,12 +1104,12 @@
       <c r="F12" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G12" s="55"/>
-      <c r="H12" s="56"/>
-      <c r="I12" s="56"/>
-      <c r="J12" s="56"/>
-      <c r="K12" s="56"/>
-      <c r="L12" s="57"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="37"/>
+      <c r="J12" s="37"/>
+      <c r="K12" s="37"/>
+      <c r="L12" s="38"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="8"/>
@@ -1207,54 +1129,54 @@
       <c r="F13" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G13" s="55"/>
-      <c r="H13" s="56"/>
-      <c r="I13" s="56"/>
-      <c r="J13" s="56"/>
-      <c r="K13" s="56"/>
-      <c r="L13" s="57"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="37"/>
+      <c r="K13" s="37"/>
+      <c r="L13" s="38"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="8"/>
       <c r="F14" s="9"/>
-      <c r="G14" s="55"/>
-      <c r="H14" s="56"/>
-      <c r="I14" s="56"/>
-      <c r="J14" s="56"/>
-      <c r="K14" s="56"/>
-      <c r="L14" s="57"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="37"/>
+      <c r="K14" s="37"/>
+      <c r="L14" s="38"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="8"/>
       <c r="F15" s="9"/>
-      <c r="G15" s="55"/>
-      <c r="H15" s="56"/>
-      <c r="I15" s="56"/>
-      <c r="J15" s="56"/>
-      <c r="K15" s="56"/>
-      <c r="L15" s="57"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="37"/>
+      <c r="J15" s="37"/>
+      <c r="K15" s="37"/>
+      <c r="L15" s="38"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="8"/>
       <c r="F16" s="9"/>
-      <c r="G16" s="55"/>
-      <c r="H16" s="56"/>
-      <c r="I16" s="56"/>
-      <c r="J16" s="56"/>
-      <c r="K16" s="56"/>
-      <c r="L16" s="57"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="37"/>
+      <c r="J16" s="37"/>
+      <c r="K16" s="37"/>
+      <c r="L16" s="38"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>18</v>
       </c>
       <c r="F17" s="9"/>
-      <c r="G17" s="55"/>
-      <c r="H17" s="56"/>
-      <c r="I17" s="56"/>
-      <c r="J17" s="56"/>
-      <c r="K17" s="56"/>
-      <c r="L17" s="57"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="37"/>
+      <c r="K17" s="37"/>
+      <c r="L17" s="38"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
@@ -1273,12 +1195,12 @@
         <v>10</v>
       </c>
       <c r="F18" s="9"/>
-      <c r="G18" s="55"/>
-      <c r="H18" s="56"/>
-      <c r="I18" s="56"/>
-      <c r="J18" s="56"/>
-      <c r="K18" s="56"/>
-      <c r="L18" s="57"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="37"/>
+      <c r="J18" s="37"/>
+      <c r="K18" s="37"/>
+      <c r="L18" s="38"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="12">
@@ -1300,60 +1222,60 @@
       <c r="F19" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G19" s="55"/>
-      <c r="H19" s="56"/>
-      <c r="I19" s="56"/>
-      <c r="J19" s="56"/>
-      <c r="K19" s="56"/>
-      <c r="L19" s="57"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
+      <c r="K19" s="37"/>
+      <c r="L19" s="38"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="8"/>
       <c r="F20" s="9"/>
-      <c r="G20" s="55"/>
-      <c r="H20" s="56"/>
-      <c r="I20" s="56"/>
-      <c r="J20" s="56"/>
-      <c r="K20" s="56"/>
-      <c r="L20" s="57"/>
+      <c r="G20" s="36"/>
+      <c r="H20" s="37"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="37"/>
+      <c r="K20" s="37"/>
+      <c r="L20" s="38"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="8"/>
-      <c r="B21" s="51" t="s">
+      <c r="B21" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="51"/>
-      <c r="D21" s="51" t="s">
+      <c r="C21" s="32"/>
+      <c r="D21" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="51"/>
+      <c r="E21" s="32"/>
       <c r="F21" s="9"/>
-      <c r="G21" s="55"/>
-      <c r="H21" s="56"/>
-      <c r="I21" s="56"/>
-      <c r="J21" s="56"/>
-      <c r="K21" s="56"/>
-      <c r="L21" s="57"/>
+      <c r="G21" s="36"/>
+      <c r="H21" s="37"/>
+      <c r="I21" s="37"/>
+      <c r="J21" s="37"/>
+      <c r="K21" s="37"/>
+      <c r="L21" s="38"/>
     </row>
     <row r="22" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="14"/>
-      <c r="B22" s="61">
+      <c r="B22" s="42">
         <f>(C19-C13)/C19</f>
         <v>0.89365263335083001</v>
       </c>
-      <c r="C22" s="61"/>
-      <c r="D22" s="61">
+      <c r="C22" s="42"/>
+      <c r="D22" s="42">
         <f>D13-D19</f>
         <v>7.1407999999999997E-4</v>
       </c>
-      <c r="E22" s="61"/>
+      <c r="E22" s="42"/>
       <c r="F22" s="15"/>
-      <c r="G22" s="58"/>
-      <c r="H22" s="59"/>
-      <c r="I22" s="59"/>
-      <c r="J22" s="59"/>
-      <c r="K22" s="59"/>
-      <c r="L22" s="60"/>
+      <c r="G22" s="39"/>
+      <c r="H22" s="40"/>
+      <c r="I22" s="40"/>
+      <c r="J22" s="40"/>
+      <c r="K22" s="40"/>
+      <c r="L22" s="41"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B23" s="23"/>
@@ -1371,77 +1293,65 @@
       <c r="A24" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="51" t="s">
+      <c r="B24" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="51"/>
+      <c r="C24" s="32"/>
       <c r="D24" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F24" s="51"/>
-      <c r="G24" s="51"/>
-      <c r="H24" s="51"/>
-      <c r="I24" s="51"/>
-      <c r="J24" s="51"/>
-      <c r="K24" s="51"/>
-      <c r="L24" s="51"/>
-      <c r="M24" s="51"/>
-    </row>
-    <row r="25" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F24" s="43"/>
+      <c r="G24" s="43"/>
+      <c r="H24" s="43"/>
+      <c r="I24" s="43"/>
+      <c r="J24" s="43"/>
+      <c r="K24" s="43"/>
+      <c r="L24" s="43"/>
+      <c r="M24" s="43"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>2965705.784</v>
       </c>
-      <c r="B25" s="51">
+      <c r="B25" s="32">
         <f>0.0000009357</f>
         <v>9.3569999999999999E-7</v>
       </c>
-      <c r="C25" s="51"/>
-      <c r="F25" s="51"/>
-      <c r="G25" s="51"/>
-      <c r="H25" s="51"/>
-      <c r="I25" s="51"/>
-      <c r="J25" s="51"/>
-      <c r="K25" s="51"/>
-      <c r="L25" s="51"/>
-      <c r="M25" s="51"/>
-    </row>
-    <row r="26" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C25" s="32"/>
+      <c r="F25" s="43"/>
+      <c r="G25" s="43"/>
+      <c r="H25" s="43"/>
+      <c r="I25" s="43"/>
+      <c r="J25" s="43"/>
+      <c r="K25" s="43"/>
+      <c r="L25" s="43"/>
+      <c r="M25" s="43"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="30">
         <f>A25*B25</f>
         <v>2.7750109020888001</v>
       </c>
-      <c r="F26" s="62"/>
-      <c r="G26" s="35" t="s">
-        <v>19</v>
-      </c>
-      <c r="H26" s="40"/>
-      <c r="I26" s="40"/>
-      <c r="J26" s="40"/>
-      <c r="K26" s="40"/>
-      <c r="L26" s="33"/>
-      <c r="M26" s="63"/>
-    </row>
-    <row r="27" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F27" s="62"/>
-      <c r="G27" s="36" t="s">
-        <v>12</v>
-      </c>
-      <c r="H27" s="40" t="s">
-        <v>22</v>
-      </c>
-      <c r="I27" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="J27" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="K27" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="L27" s="33"/>
-      <c r="M27" s="63"/>
-    </row>
-    <row r="28" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F26" s="43"/>
+      <c r="G26" s="44"/>
+      <c r="H26" s="45"/>
+      <c r="I26" s="45"/>
+      <c r="J26" s="45"/>
+      <c r="K26" s="45"/>
+      <c r="L26" s="45"/>
+      <c r="M26" s="46"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="F27" s="43"/>
+      <c r="G27" s="47"/>
+      <c r="H27" s="45"/>
+      <c r="I27" s="45"/>
+      <c r="J27" s="45"/>
+      <c r="K27" s="45"/>
+      <c r="L27" s="45"/>
+      <c r="M27" s="46"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>27</v>
       </c>
@@ -1457,29 +1367,16 @@
       <c r="E28" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F28" s="62"/>
-      <c r="G28" s="37">
-        <v>949430</v>
-      </c>
-      <c r="H28" s="41">
-        <v>7.8499999999999994E-6</v>
-      </c>
-      <c r="I28" s="44">
-        <f t="shared" ref="I28:I33" si="2">$A$8*H28</f>
-        <v>7.453025499999999</v>
-      </c>
-      <c r="J28" s="44">
-        <v>1.8736E-4</v>
-      </c>
-      <c r="K28" s="44">
-        <v>1.7786999999999999</v>
-      </c>
-      <c r="L28" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="M28" s="63"/>
-    </row>
-    <row r="29" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F28" s="43"/>
+      <c r="G28" s="48"/>
+      <c r="H28" s="49"/>
+      <c r="I28" s="50"/>
+      <c r="J28" s="50"/>
+      <c r="K28" s="50"/>
+      <c r="L28" s="50"/>
+      <c r="M28" s="46"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <f>C29+E29*TAN(RADIANS(B29))+2*D29/COS(RADIANS(B29))</f>
         <v>93.069200243157383</v>
@@ -1496,47 +1393,29 @@
       <c r="E29" s="1">
         <v>100</v>
       </c>
-      <c r="F29" s="62"/>
-      <c r="G29" s="38"/>
-      <c r="H29" s="42">
-        <v>2.7700000000000002E-6</v>
-      </c>
-      <c r="I29" s="45">
-        <f t="shared" si="2"/>
-        <v>2.6299211000000002</v>
-      </c>
-      <c r="J29" s="40">
-        <v>5.3541999999999999E-4</v>
-      </c>
-      <c r="K29" s="40">
-        <v>1.7766</v>
-      </c>
-      <c r="L29" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="M29" s="63"/>
-    </row>
-    <row r="30" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F29" s="43"/>
+      <c r="G29" s="51"/>
+      <c r="H29" s="52"/>
+      <c r="I29" s="45"/>
+      <c r="J29" s="45"/>
+      <c r="K29" s="45"/>
+      <c r="L29" s="45"/>
+      <c r="M29" s="46"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E30" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F30" s="62"/>
-      <c r="G30" s="36"/>
-      <c r="H30" s="42">
-        <v>8.3000000000000002E-6</v>
-      </c>
-      <c r="I30" s="40">
-        <f t="shared" si="2"/>
-        <v>7.8802690000000002</v>
-      </c>
-      <c r="J30" s="40"/>
-      <c r="K30" s="40"/>
-      <c r="L30" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="M30" s="63"/>
-    </row>
-    <row r="31" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F30" s="43"/>
+      <c r="G30" s="47"/>
+      <c r="H30" s="52"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
+      <c r="K30" s="45"/>
+      <c r="L30" s="45"/>
+      <c r="M30" s="46"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <f>A29*E31</f>
         <v>116.33650030394674</v>
@@ -1544,167 +1423,107 @@
       <c r="E31" s="1">
         <v>1.25</v>
       </c>
-      <c r="F31" s="62"/>
-      <c r="G31" s="36"/>
-      <c r="H31" s="42">
-        <v>4.6199999999999998E-6</v>
-      </c>
-      <c r="I31" s="45">
-        <f t="shared" si="2"/>
-        <v>4.3863665999999997</v>
-      </c>
-      <c r="J31" s="40">
-        <v>4.0146000000000002E-4</v>
-      </c>
-      <c r="K31" s="40">
-        <v>1.7738</v>
-      </c>
-      <c r="L31" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="M31" s="63"/>
-    </row>
-    <row r="32" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F32" s="62"/>
-      <c r="G32" s="36"/>
-      <c r="H32" s="42">
-        <v>7.7500000000000003E-6</v>
-      </c>
-      <c r="I32" s="40">
-        <f t="shared" si="2"/>
-        <v>7.3580825000000001</v>
-      </c>
-      <c r="J32" s="40"/>
-      <c r="K32" s="40"/>
-      <c r="L32" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="M32" s="63"/>
-    </row>
-    <row r="33" spans="6:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F33" s="62"/>
-      <c r="G33" s="39"/>
-      <c r="H33" s="43">
-        <v>1.7999999999999999E-6</v>
-      </c>
-      <c r="I33" s="46">
-        <f t="shared" si="2"/>
-        <v>1.708974</v>
-      </c>
-      <c r="J33" s="47">
-        <v>8.5260999999999996E-4</v>
-      </c>
-      <c r="K33" s="47">
-        <v>1.7747999999999999</v>
-      </c>
-      <c r="L33" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="M33" s="63"/>
+      <c r="F31" s="43"/>
+      <c r="G31" s="47"/>
+      <c r="H31" s="52"/>
+      <c r="I31" s="45"/>
+      <c r="J31" s="45"/>
+      <c r="K31" s="45"/>
+      <c r="L31" s="45"/>
+      <c r="M31" s="46"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="F32" s="43"/>
+      <c r="G32" s="47"/>
+      <c r="H32" s="52"/>
+      <c r="I32" s="45"/>
+      <c r="J32" s="45"/>
+      <c r="K32" s="45"/>
+      <c r="L32" s="45"/>
+      <c r="M32" s="46"/>
+    </row>
+    <row r="33" spans="6:13" x14ac:dyDescent="0.3">
+      <c r="F33" s="43"/>
+      <c r="G33" s="47"/>
+      <c r="H33" s="52"/>
+      <c r="I33" s="45"/>
+      <c r="J33" s="50"/>
+      <c r="K33" s="50"/>
+      <c r="L33" s="50"/>
+      <c r="M33" s="46"/>
     </row>
     <row r="34" spans="6:13" x14ac:dyDescent="0.3">
-      <c r="F34" s="51"/>
-      <c r="G34" s="51"/>
-      <c r="H34" s="51"/>
-      <c r="I34" s="51"/>
-      <c r="J34" s="51"/>
-      <c r="K34" s="51"/>
-      <c r="L34" s="51"/>
-      <c r="M34" s="51"/>
-    </row>
-    <row r="35" spans="6:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F35" s="51"/>
-      <c r="G35" s="51"/>
-      <c r="H35" s="51"/>
-      <c r="I35" s="51"/>
-      <c r="J35" s="51"/>
-      <c r="K35" s="51"/>
-      <c r="L35" s="51"/>
-      <c r="M35" s="51"/>
-    </row>
-    <row r="36" spans="6:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F36" s="62"/>
-      <c r="G36" s="35" t="s">
-        <v>18</v>
-      </c>
-      <c r="H36" s="40"/>
-      <c r="I36" s="40"/>
-      <c r="J36" s="40"/>
-      <c r="K36" s="40"/>
-      <c r="L36" s="33"/>
-      <c r="M36" s="63"/>
-    </row>
-    <row r="37" spans="6:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F37" s="62"/>
-      <c r="G37" s="36" t="s">
-        <v>12</v>
-      </c>
-      <c r="H37" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="I37" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="J37" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="K37" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="L37" s="33"/>
-      <c r="M37" s="63"/>
-    </row>
-    <row r="38" spans="6:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F38" s="62"/>
-      <c r="G38" s="49">
-        <v>2047100</v>
-      </c>
-      <c r="H38" s="43">
-        <v>7.8499999999999994E-6</v>
-      </c>
-      <c r="I38" s="50">
-        <f>$A$19*H38</f>
-        <v>16.069734999999998</v>
-      </c>
-      <c r="J38" s="50">
-        <v>1.3852999999999999E-4</v>
-      </c>
-      <c r="K38" s="50">
-        <v>1.5971</v>
-      </c>
-      <c r="L38" s="48" t="s">
-        <v>11</v>
-      </c>
-      <c r="M38" s="63"/>
+      <c r="F34" s="43"/>
+      <c r="G34" s="43"/>
+      <c r="H34" s="43"/>
+      <c r="I34" s="43"/>
+      <c r="J34" s="43"/>
+      <c r="K34" s="43"/>
+      <c r="L34" s="43"/>
+      <c r="M34" s="43"/>
+    </row>
+    <row r="35" spans="6:13" x14ac:dyDescent="0.3">
+      <c r="F35" s="43"/>
+      <c r="G35" s="43"/>
+      <c r="H35" s="43"/>
+      <c r="I35" s="43"/>
+      <c r="J35" s="43"/>
+      <c r="K35" s="43"/>
+      <c r="L35" s="43"/>
+      <c r="M35" s="43"/>
+    </row>
+    <row r="36" spans="6:13" x14ac:dyDescent="0.3">
+      <c r="F36" s="43"/>
+      <c r="G36" s="44"/>
+      <c r="H36" s="45"/>
+      <c r="I36" s="45"/>
+      <c r="J36" s="45"/>
+      <c r="K36" s="45"/>
+      <c r="L36" s="45"/>
+      <c r="M36" s="46"/>
+    </row>
+    <row r="37" spans="6:13" x14ac:dyDescent="0.3">
+      <c r="F37" s="43"/>
+      <c r="G37" s="47"/>
+      <c r="H37" s="45"/>
+      <c r="I37" s="45"/>
+      <c r="J37" s="45"/>
+      <c r="K37" s="45"/>
+      <c r="L37" s="45"/>
+      <c r="M37" s="46"/>
+    </row>
+    <row r="38" spans="6:13" x14ac:dyDescent="0.3">
+      <c r="F38" s="43"/>
+      <c r="G38" s="51"/>
+      <c r="H38" s="52"/>
+      <c r="I38" s="45"/>
+      <c r="J38" s="45"/>
+      <c r="K38" s="45"/>
+      <c r="L38" s="50"/>
+      <c r="M38" s="46"/>
     </row>
     <row r="39" spans="6:13" x14ac:dyDescent="0.3">
-      <c r="F39" s="51"/>
-      <c r="G39" s="51"/>
-      <c r="H39" s="51"/>
-      <c r="I39" s="51"/>
-      <c r="J39" s="51"/>
-      <c r="K39" s="51"/>
-      <c r="L39" s="51"/>
-      <c r="M39" s="51"/>
+      <c r="F39" s="32"/>
+      <c r="G39" s="32"/>
+      <c r="H39" s="32"/>
+      <c r="I39" s="32"/>
+      <c r="J39" s="32"/>
+      <c r="K39" s="32"/>
+      <c r="L39" s="32"/>
+      <c r="M39" s="32"/>
     </row>
     <row r="40" spans="6:13" x14ac:dyDescent="0.3">
-      <c r="F40" s="51"/>
-      <c r="G40" s="51"/>
-      <c r="H40" s="51"/>
-      <c r="I40" s="51"/>
-      <c r="J40" s="51"/>
-      <c r="K40" s="51"/>
-      <c r="L40" s="51"/>
-      <c r="M40" s="51"/>
+      <c r="F40" s="32"/>
+      <c r="G40" s="32"/>
+      <c r="H40" s="32"/>
+      <c r="I40" s="32"/>
+      <c r="J40" s="32"/>
+      <c r="K40" s="32"/>
+      <c r="L40" s="32"/>
+      <c r="M40" s="32"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="F39:M40"/>
-    <mergeCell ref="F26:F33"/>
-    <mergeCell ref="M26:M33"/>
-    <mergeCell ref="F34:M35"/>
-    <mergeCell ref="F36:F38"/>
-    <mergeCell ref="M36:M38"/>
+  <mergeCells count="8">
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="G5:L22"/>
@@ -1712,7 +1531,7 @@
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B22:C22"/>
-    <mergeCell ref="F24:M25"/>
+    <mergeCell ref="F39:M40"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update Box and Lid Combination Word Document and Datasheet
</commit_message>
<xml_diff>
--- a/Documents/Box and Lid Combination/Box and Lid Combination Data Sheet.xlsx
+++ b/Documents/Box and Lid Combination/Box and Lid Combination Data Sheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GTIIT\Semester 6_Spring 2024\design_project_github\Project-in-Design-2024\Documents\Box and Lid Combination\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GTIIT\Semester 6_Spring 2024\Design project\Box and Lid Combination\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE229DE1-DA22-488E-A542-E0E8288FC7D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13FBC5C9-71C1-4EA7-907E-C854F7B3E9F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="48">
   <si>
     <t>Motor mass [kg]</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -147,10 +147,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Shaft coupling [kg]</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>density of pipe beam [kg/mm^3]</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -184,6 +180,70 @@
   </si>
   <si>
     <t>safety factor</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>flange</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>volume [mm^3]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>density [kg/mm^3]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>mass [kg]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Flange mass [kg]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Final for </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Final</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>max x [mm]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>avg x [mm]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>avg stress [MPa]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Max Stress [MPa]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>max stress [MPa]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vertical deviation percentage %</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Box coupling [kg]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Power coupling [kg]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Volume Reduction</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -191,7 +251,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,8 +279,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -239,14 +304,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -334,11 +393,52 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -376,9 +476,6 @@
     <xf numFmtId="11" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -400,92 +497,113 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -834,8 +952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -867,13 +985,17 @@
         <v>6</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="29"/>
+        <v>45</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
@@ -896,81 +1018,92 @@
         <v>5.3194430700000002</v>
       </c>
       <c r="G2" s="2">
-        <v>1.8846999999999999E-2</v>
-      </c>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="21"/>
+        <v>0.5</v>
+      </c>
+      <c r="H2" s="2">
+        <f>C35</f>
+        <v>0.14787648601</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="8"/>
       <c r="G3" s="2"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="21"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
     </row>
     <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="16">
+      <c r="B4" s="15">
         <f>$A$2*B2</f>
         <v>12.50775</v>
       </c>
-      <c r="C4" s="16">
+      <c r="C4" s="15">
         <f t="shared" ref="C4:E4" si="0">$A$2*C2</f>
         <v>0.88434207000000009</v>
       </c>
-      <c r="D4" s="16">
+      <c r="D4" s="15">
         <f t="shared" si="0"/>
         <v>0.86426100000000006</v>
       </c>
-      <c r="E4" s="16">
+      <c r="E4" s="15">
         <f t="shared" si="0"/>
         <v>3.57084</v>
       </c>
-      <c r="F4" s="16"/>
+      <c r="F4" s="15"/>
       <c r="G4" s="4">
         <f>$A$2*G2</f>
-        <v>0.18488906999999999</v>
-      </c>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="22"/>
+        <v>4.9050000000000002</v>
+      </c>
+      <c r="H4" s="4">
+        <f>$A$2*H2</f>
+        <v>1.4506683277581001</v>
+      </c>
+      <c r="I4" s="4">
+        <f>$A$2*I2</f>
+        <v>1.1772</v>
+      </c>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="18"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
+      <c r="A5" s="17"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
       <c r="F5" s="7"/>
-      <c r="G5" s="33" t="e" vm="1">
+      <c r="G5" s="47" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="H5" s="34"/>
-      <c r="I5" s="34"/>
-      <c r="J5" s="34"/>
-      <c r="K5" s="34"/>
-      <c r="L5" s="35"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="48"/>
+      <c r="K5" s="48"/>
+      <c r="L5" s="49"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>19</v>
       </c>
       <c r="F6" s="9"/>
-      <c r="G6" s="36"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="37"/>
-      <c r="K6" s="37"/>
-      <c r="L6" s="38"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="51"/>
+      <c r="J6" s="51"/>
+      <c r="K6" s="51"/>
+      <c r="L6" s="52"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
@@ -986,71 +1119,71 @@
         <v>9</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="F7" s="9"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="37"/>
-      <c r="J7" s="37"/>
-      <c r="K7" s="37"/>
-      <c r="L7" s="38"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="51"/>
+      <c r="I7" s="51"/>
+      <c r="J7" s="51"/>
+      <c r="K7" s="51"/>
+      <c r="L7" s="52"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="31">
+      <c r="A8" s="43">
         <v>949430</v>
       </c>
-      <c r="B8" s="25">
+      <c r="B8" s="20">
         <v>7.8499999999999994E-6</v>
       </c>
-      <c r="C8" s="23">
-        <f t="shared" ref="C8:C13" si="1">$A$8*B8</f>
+      <c r="C8" s="20">
+        <f t="shared" ref="C8:C12" si="1">$A$8*B8</f>
         <v>7.453025499999999</v>
       </c>
-      <c r="D8" s="23">
-        <v>1.8736E-4</v>
-      </c>
-      <c r="E8" s="23">
-        <v>1.7786999999999999</v>
+      <c r="D8" s="20">
+        <v>2.6435E-4</v>
+      </c>
+      <c r="E8" s="20">
+        <v>1.6995</v>
       </c>
       <c r="F8" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="36"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
-      <c r="J8" s="37"/>
-      <c r="K8" s="37"/>
-      <c r="L8" s="38"/>
+      <c r="G8" s="50"/>
+      <c r="H8" s="51"/>
+      <c r="I8" s="51"/>
+      <c r="J8" s="51"/>
+      <c r="K8" s="51"/>
+      <c r="L8" s="52"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="12"/>
-      <c r="B9" s="26">
+      <c r="B9" s="1">
         <v>2.7700000000000002E-6</v>
       </c>
-      <c r="C9" s="27">
+      <c r="C9" s="22">
         <f t="shared" si="1"/>
         <v>2.6299211000000002</v>
       </c>
       <c r="D9" s="1">
-        <v>5.3541999999999999E-4</v>
+        <v>7.4691999999999998E-4</v>
       </c>
       <c r="E9" s="1">
-        <v>1.7766</v>
+        <v>1.6866000000000001</v>
       </c>
       <c r="F9" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="36"/>
-      <c r="H9" s="37"/>
-      <c r="I9" s="37"/>
-      <c r="J9" s="37"/>
-      <c r="K9" s="37"/>
-      <c r="L9" s="38"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="51"/>
+      <c r="I9" s="51"/>
+      <c r="J9" s="51"/>
+      <c r="K9" s="51"/>
+      <c r="L9" s="52"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="8"/>
-      <c r="B10" s="26">
+      <c r="B10" s="1">
         <v>8.3000000000000002E-6</v>
       </c>
       <c r="C10" s="1">
@@ -1060,41 +1193,41 @@
       <c r="F10" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="36"/>
-      <c r="H10" s="37"/>
-      <c r="I10" s="37"/>
-      <c r="J10" s="37"/>
-      <c r="K10" s="37"/>
-      <c r="L10" s="38"/>
+      <c r="G10" s="50"/>
+      <c r="H10" s="51"/>
+      <c r="I10" s="51"/>
+      <c r="J10" s="51"/>
+      <c r="K10" s="51"/>
+      <c r="L10" s="52"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="8"/>
-      <c r="B11" s="26">
+      <c r="B11" s="1">
         <v>4.6199999999999998E-6</v>
       </c>
-      <c r="C11" s="27">
+      <c r="C11" s="22">
         <f t="shared" si="1"/>
         <v>4.3863665999999997</v>
       </c>
       <c r="D11" s="1">
-        <v>4.0146000000000002E-4</v>
+        <v>5.5371000000000001E-4</v>
       </c>
       <c r="E11" s="1">
-        <v>1.7738</v>
+        <v>1.6727000000000001</v>
       </c>
       <c r="F11" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="36"/>
-      <c r="H11" s="37"/>
-      <c r="I11" s="37"/>
-      <c r="J11" s="37"/>
-      <c r="K11" s="37"/>
-      <c r="L11" s="38"/>
+      <c r="G11" s="50"/>
+      <c r="H11" s="51"/>
+      <c r="I11" s="51"/>
+      <c r="J11" s="51"/>
+      <c r="K11" s="51"/>
+      <c r="L11" s="52"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="8"/>
-      <c r="B12" s="26">
+      <c r="B12" s="1">
         <v>7.7500000000000003E-6</v>
       </c>
       <c r="C12" s="1">
@@ -1104,79 +1237,113 @@
       <c r="F12" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G12" s="36"/>
-      <c r="H12" s="37"/>
-      <c r="I12" s="37"/>
-      <c r="J12" s="37"/>
-      <c r="K12" s="37"/>
-      <c r="L12" s="38"/>
+      <c r="G12" s="50"/>
+      <c r="H12" s="51"/>
+      <c r="I12" s="51"/>
+      <c r="J12" s="51"/>
+      <c r="K12" s="51"/>
+      <c r="L12" s="52"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="8"/>
-      <c r="B13" s="26">
+      <c r="B13" s="1">
         <v>1.7999999999999999E-6</v>
       </c>
-      <c r="C13" s="27">
-        <f t="shared" si="1"/>
+      <c r="C13" s="22">
+        <f>$A$8*B13</f>
         <v>1.708974</v>
       </c>
-      <c r="D13" s="24">
-        <v>8.5260999999999996E-4</v>
-      </c>
-      <c r="E13" s="24">
-        <v>1.7747999999999999</v>
-      </c>
-      <c r="F13" s="13" t="s">
+      <c r="D13" s="1">
+        <v>1.1804000000000001E-3</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1.6774</v>
+      </c>
+      <c r="F13" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="G13" s="36"/>
-      <c r="H13" s="37"/>
-      <c r="I13" s="37"/>
-      <c r="J13" s="37"/>
-      <c r="K13" s="37"/>
-      <c r="L13" s="38"/>
+      <c r="G13" s="50"/>
+      <c r="H13" s="51"/>
+      <c r="I13" s="51"/>
+      <c r="J13" s="51"/>
+      <c r="K13" s="51"/>
+      <c r="L13" s="52"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="8"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="37"/>
-      <c r="I14" s="37"/>
-      <c r="J14" s="37"/>
-      <c r="K14" s="37"/>
-      <c r="L14" s="38"/>
+      <c r="A14" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G14" s="50"/>
+      <c r="H14" s="51"/>
+      <c r="I14" s="51"/>
+      <c r="J14" s="51"/>
+      <c r="K14" s="51"/>
+      <c r="L14" s="52"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="8"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="37"/>
-      <c r="J15" s="37"/>
-      <c r="K15" s="37"/>
-      <c r="L15" s="38"/>
+      <c r="B15" s="1">
+        <f>D9</f>
+        <v>7.4691999999999998E-4</v>
+      </c>
+      <c r="C15" s="1">
+        <f>0.00018306</f>
+        <v>1.8306E-4</v>
+      </c>
+      <c r="D15" s="1">
+        <f>E9</f>
+        <v>1.6866000000000001</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0.14297000000000001</v>
+      </c>
+      <c r="F15" s="9">
+        <f>B15/95*100</f>
+        <v>7.8623157894736843E-4</v>
+      </c>
+      <c r="G15" s="50"/>
+      <c r="H15" s="51"/>
+      <c r="I15" s="51"/>
+      <c r="J15" s="51"/>
+      <c r="K15" s="51"/>
+      <c r="L15" s="52"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="8"/>
       <c r="F16" s="9"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="37"/>
-      <c r="J16" s="37"/>
-      <c r="K16" s="37"/>
-      <c r="L16" s="38"/>
+      <c r="G16" s="50"/>
+      <c r="H16" s="51"/>
+      <c r="I16" s="51"/>
+      <c r="J16" s="51"/>
+      <c r="K16" s="51"/>
+      <c r="L16" s="52"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>18</v>
       </c>
       <c r="F17" s="9"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="37"/>
-      <c r="I17" s="37"/>
-      <c r="J17" s="37"/>
-      <c r="K17" s="37"/>
-      <c r="L17" s="38"/>
+      <c r="G17" s="50"/>
+      <c r="H17" s="51"/>
+      <c r="I17" s="51"/>
+      <c r="J17" s="51"/>
+      <c r="K17" s="51"/>
+      <c r="L17" s="52"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
@@ -1195,18 +1362,18 @@
         <v>10</v>
       </c>
       <c r="F18" s="9"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="37"/>
-      <c r="I18" s="37"/>
-      <c r="J18" s="37"/>
-      <c r="K18" s="37"/>
-      <c r="L18" s="38"/>
+      <c r="G18" s="50"/>
+      <c r="H18" s="51"/>
+      <c r="I18" s="51"/>
+      <c r="J18" s="51"/>
+      <c r="K18" s="51"/>
+      <c r="L18" s="52"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" s="12">
+      <c r="A19" s="8">
         <v>2047100</v>
       </c>
-      <c r="B19" s="26">
+      <c r="B19" s="21">
         <v>7.8499999999999994E-6</v>
       </c>
       <c r="C19" s="1">
@@ -1222,163 +1389,193 @@
       <c r="F19" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G19" s="36"/>
-      <c r="H19" s="37"/>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
-      <c r="K19" s="37"/>
-      <c r="L19" s="38"/>
+      <c r="G19" s="50"/>
+      <c r="H19" s="51"/>
+      <c r="I19" s="51"/>
+      <c r="J19" s="51"/>
+      <c r="K19" s="51"/>
+      <c r="L19" s="52"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="8"/>
       <c r="F20" s="9"/>
-      <c r="G20" s="36"/>
-      <c r="H20" s="37"/>
-      <c r="I20" s="37"/>
-      <c r="J20" s="37"/>
-      <c r="K20" s="37"/>
-      <c r="L20" s="38"/>
+      <c r="G20" s="50"/>
+      <c r="H20" s="51"/>
+      <c r="I20" s="51"/>
+      <c r="J20" s="51"/>
+      <c r="K20" s="51"/>
+      <c r="L20" s="52"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21" s="8"/>
-      <c r="B21" s="32" t="s">
+      <c r="A21" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="32"/>
-      <c r="D21" s="32" t="s">
+      <c r="C21" s="44"/>
+      <c r="D21" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="32"/>
+      <c r="E21" s="44"/>
       <c r="F21" s="9"/>
-      <c r="G21" s="36"/>
-      <c r="H21" s="37"/>
-      <c r="I21" s="37"/>
-      <c r="J21" s="37"/>
-      <c r="K21" s="37"/>
-      <c r="L21" s="38"/>
+      <c r="G21" s="50"/>
+      <c r="H21" s="51"/>
+      <c r="I21" s="51"/>
+      <c r="J21" s="51"/>
+      <c r="K21" s="51"/>
+      <c r="L21" s="52"/>
     </row>
     <row r="22" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="14"/>
-      <c r="B22" s="42">
-        <f>(C19-C13)/C19</f>
-        <v>0.89365263335083001</v>
-      </c>
-      <c r="C22" s="42"/>
-      <c r="D22" s="42">
+      <c r="A22" s="13">
+        <f>(A19-A8)/A19</f>
+        <v>0.53620731766889751</v>
+      </c>
+      <c r="B22" s="56">
+        <f>(C19-C9)/C19</f>
+        <v>0.8363432191009994</v>
+      </c>
+      <c r="C22" s="56"/>
+      <c r="D22" s="56">
         <f>D13-D19</f>
-        <v>7.1407999999999997E-4</v>
-      </c>
-      <c r="E22" s="42"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="40"/>
-      <c r="I22" s="40"/>
-      <c r="J22" s="40"/>
-      <c r="K22" s="40"/>
-      <c r="L22" s="41"/>
+        <v>1.0418700000000001E-3</v>
+      </c>
+      <c r="E22" s="56"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="53"/>
+      <c r="H22" s="54"/>
+      <c r="I22" s="54"/>
+      <c r="J22" s="54"/>
+      <c r="K22" s="54"/>
+      <c r="L22" s="55"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B23" s="23"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="20"/>
-      <c r="K23" s="20"/>
-      <c r="L23" s="20"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="19"/>
+      <c r="K23" s="19"/>
+      <c r="L23" s="19"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="44"/>
+      <c r="D24" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" s="32"/>
-      <c r="D24" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F24" s="43"/>
-      <c r="G24" s="43"/>
-      <c r="H24" s="43"/>
-      <c r="I24" s="43"/>
-      <c r="J24" s="43"/>
-      <c r="K24" s="43"/>
-      <c r="L24" s="43"/>
-      <c r="M24" s="43"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="F24" s="44"/>
+      <c r="G24" s="44"/>
+      <c r="H24" s="44"/>
+      <c r="I24" s="44"/>
+      <c r="J24" s="44"/>
+      <c r="K24" s="44"/>
+      <c r="L24" s="44"/>
+      <c r="M24" s="44"/>
+    </row>
+    <row r="25" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>2965705.784</v>
       </c>
-      <c r="B25" s="32">
+      <c r="B25" s="44">
         <f>0.0000009357</f>
         <v>9.3569999999999999E-7</v>
       </c>
-      <c r="C25" s="32"/>
-      <c r="F25" s="43"/>
-      <c r="G25" s="43"/>
-      <c r="H25" s="43"/>
-      <c r="I25" s="43"/>
-      <c r="J25" s="43"/>
-      <c r="K25" s="43"/>
-      <c r="L25" s="43"/>
-      <c r="M25" s="43"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A26" s="30">
+      <c r="C25" s="44"/>
+      <c r="F25" s="44"/>
+      <c r="G25" s="44"/>
+      <c r="H25" s="44"/>
+      <c r="I25" s="44"/>
+      <c r="J25" s="44"/>
+      <c r="K25" s="44"/>
+      <c r="L25" s="44"/>
+      <c r="M25" s="44"/>
+    </row>
+    <row r="26" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="24">
         <f>A25*B25</f>
         <v>2.7750109020888001</v>
       </c>
-      <c r="F26" s="43"/>
-      <c r="G26" s="44"/>
-      <c r="H26" s="45"/>
-      <c r="I26" s="45"/>
-      <c r="J26" s="45"/>
-      <c r="K26" s="45"/>
-      <c r="L26" s="45"/>
+      <c r="F26" s="45"/>
+      <c r="G26" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="H26" s="32"/>
+      <c r="I26" s="32"/>
+      <c r="J26" s="32"/>
+      <c r="K26" s="32"/>
+      <c r="L26" s="25"/>
       <c r="M26" s="46"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="F27" s="43"/>
-      <c r="G27" s="47"/>
-      <c r="H27" s="45"/>
-      <c r="I27" s="45"/>
-      <c r="J27" s="45"/>
-      <c r="K27" s="45"/>
-      <c r="L27" s="45"/>
+    <row r="27" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F27" s="45"/>
+      <c r="G27" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="H27" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="I27" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="J27" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K27" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="L27" s="25"/>
       <c r="M27" s="46"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E28" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F28" s="43"/>
-      <c r="G28" s="48"/>
-      <c r="H28" s="49"/>
-      <c r="I28" s="50"/>
-      <c r="J28" s="50"/>
-      <c r="K28" s="50"/>
-      <c r="L28" s="50"/>
+      <c r="F28" s="45"/>
+      <c r="G28" s="29">
+        <v>949430</v>
+      </c>
+      <c r="H28" s="33">
+        <v>7.8499999999999994E-6</v>
+      </c>
+      <c r="I28" s="36">
+        <f t="shared" ref="I28:I33" si="2">$A$8*H28</f>
+        <v>7.453025499999999</v>
+      </c>
+      <c r="J28" s="36">
+        <v>2.6435E-4</v>
+      </c>
+      <c r="K28" s="26">
+        <v>1.6995</v>
+      </c>
+      <c r="L28" s="26" t="s">
+        <v>11</v>
+      </c>
       <c r="M28" s="46"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
-        <f>C29+E29*TAN(RADIANS(B29))+2*D29/COS(RADIANS(B29))</f>
+        <f>C29+E29*TAN(RADIANS(B29))+D29/COS(RADIANS(B29))</f>
         <v>93.069200243157383</v>
       </c>
       <c r="B29" s="1">
@@ -1388,34 +1585,52 @@
         <v>30</v>
       </c>
       <c r="D29" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E29" s="1">
         <v>100</v>
       </c>
-      <c r="F29" s="43"/>
-      <c r="G29" s="51"/>
-      <c r="H29" s="52"/>
-      <c r="I29" s="45"/>
-      <c r="J29" s="45"/>
-      <c r="K29" s="45"/>
-      <c r="L29" s="45"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="34">
+        <v>2.7700000000000002E-6</v>
+      </c>
+      <c r="I29" s="37">
+        <f t="shared" si="2"/>
+        <v>2.6299211000000002</v>
+      </c>
+      <c r="J29" s="32">
+        <v>7.4691999999999998E-4</v>
+      </c>
+      <c r="K29" s="25">
+        <v>1.6866000000000001</v>
+      </c>
+      <c r="L29" s="25" t="s">
+        <v>13</v>
+      </c>
       <c r="M29" s="46"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E30" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F30" s="43"/>
-      <c r="G30" s="47"/>
-      <c r="H30" s="52"/>
-      <c r="I30" s="45"/>
-      <c r="J30" s="45"/>
-      <c r="K30" s="45"/>
-      <c r="L30" s="45"/>
+        <v>31</v>
+      </c>
+      <c r="F30" s="45"/>
+      <c r="G30" s="28"/>
+      <c r="H30" s="34">
+        <v>8.3000000000000002E-6</v>
+      </c>
+      <c r="I30" s="32">
+        <f t="shared" si="2"/>
+        <v>7.8802690000000002</v>
+      </c>
+      <c r="J30" s="32"/>
+      <c r="K30" s="25"/>
+      <c r="L30" s="25" t="s">
+        <v>14</v>
+      </c>
       <c r="M30" s="46"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <f>A29*E31</f>
         <v>116.33650030394674</v>
@@ -1423,107 +1638,186 @@
       <c r="E31" s="1">
         <v>1.25</v>
       </c>
-      <c r="F31" s="43"/>
-      <c r="G31" s="47"/>
-      <c r="H31" s="52"/>
-      <c r="I31" s="45"/>
-      <c r="J31" s="45"/>
-      <c r="K31" s="45"/>
-      <c r="L31" s="45"/>
+      <c r="F31" s="45"/>
+      <c r="G31" s="28"/>
+      <c r="H31" s="34">
+        <v>4.6199999999999998E-6</v>
+      </c>
+      <c r="I31" s="37">
+        <f t="shared" si="2"/>
+        <v>4.3863665999999997</v>
+      </c>
+      <c r="J31" s="32">
+        <v>5.5371000000000001E-4</v>
+      </c>
+      <c r="K31" s="25">
+        <v>1.6727000000000001</v>
+      </c>
+      <c r="L31" s="25" t="s">
+        <v>15</v>
+      </c>
       <c r="M31" s="46"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="F32" s="43"/>
-      <c r="G32" s="47"/>
-      <c r="H32" s="52"/>
-      <c r="I32" s="45"/>
-      <c r="J32" s="45"/>
-      <c r="K32" s="45"/>
-      <c r="L32" s="45"/>
+    <row r="32" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F32" s="45"/>
+      <c r="G32" s="28"/>
+      <c r="H32" s="34">
+        <v>7.7500000000000003E-6</v>
+      </c>
+      <c r="I32" s="32">
+        <f t="shared" si="2"/>
+        <v>7.3580825000000001</v>
+      </c>
+      <c r="J32" s="32"/>
+      <c r="K32" s="25"/>
+      <c r="L32" s="25" t="s">
+        <v>16</v>
+      </c>
       <c r="M32" s="46"/>
     </row>
-    <row r="33" spans="6:13" x14ac:dyDescent="0.3">
-      <c r="F33" s="43"/>
-      <c r="G33" s="47"/>
-      <c r="H33" s="52"/>
-      <c r="I33" s="45"/>
-      <c r="J33" s="50"/>
-      <c r="K33" s="50"/>
-      <c r="L33" s="50"/>
+    <row r="33" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F33" s="45"/>
+      <c r="G33" s="31"/>
+      <c r="H33" s="35">
+        <v>1.7999999999999999E-6</v>
+      </c>
+      <c r="I33" s="38">
+        <f t="shared" si="2"/>
+        <v>1.708974</v>
+      </c>
+      <c r="J33" s="41">
+        <v>1.1804000000000001E-3</v>
+      </c>
+      <c r="K33" s="14">
+        <v>1.6774</v>
+      </c>
+      <c r="L33" s="42" t="s">
+        <v>17</v>
+      </c>
       <c r="M33" s="46"/>
     </row>
-    <row r="34" spans="6:13" x14ac:dyDescent="0.3">
-      <c r="F34" s="43"/>
-      <c r="G34" s="43"/>
-      <c r="H34" s="43"/>
-      <c r="I34" s="43"/>
-      <c r="J34" s="43"/>
-      <c r="K34" s="43"/>
-      <c r="L34" s="43"/>
-      <c r="M34" s="43"/>
-    </row>
-    <row r="35" spans="6:13" x14ac:dyDescent="0.3">
-      <c r="F35" s="43"/>
-      <c r="G35" s="43"/>
-      <c r="H35" s="43"/>
-      <c r="I35" s="43"/>
-      <c r="J35" s="43"/>
-      <c r="K35" s="43"/>
-      <c r="L35" s="43"/>
-      <c r="M35" s="43"/>
-    </row>
-    <row r="36" spans="6:13" x14ac:dyDescent="0.3">
-      <c r="F36" s="43"/>
-      <c r="G36" s="44"/>
-      <c r="H36" s="45"/>
-      <c r="I36" s="45"/>
-      <c r="J36" s="45"/>
-      <c r="K36" s="45"/>
-      <c r="L36" s="45"/>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F34" s="44"/>
+      <c r="G34" s="44"/>
+      <c r="H34" s="44"/>
+      <c r="I34" s="44"/>
+      <c r="J34" s="44"/>
+      <c r="K34" s="44"/>
+      <c r="L34" s="44"/>
+      <c r="M34" s="44"/>
+    </row>
+    <row r="35" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="2">
+        <v>53385.012999999999</v>
+      </c>
+      <c r="B35" s="21">
+        <v>2.7700000000000002E-6</v>
+      </c>
+      <c r="C35" s="21">
+        <f>A35*B35</f>
+        <v>0.14787648601</v>
+      </c>
+      <c r="F35" s="44"/>
+      <c r="G35" s="44"/>
+      <c r="H35" s="44"/>
+      <c r="I35" s="44"/>
+      <c r="J35" s="44"/>
+      <c r="K35" s="44"/>
+      <c r="L35" s="44"/>
+      <c r="M35" s="44"/>
+    </row>
+    <row r="36" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F36" s="45"/>
+      <c r="G36" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="H36" s="32"/>
+      <c r="I36" s="32"/>
+      <c r="J36" s="32"/>
+      <c r="K36" s="32"/>
+      <c r="L36" s="25"/>
       <c r="M36" s="46"/>
     </row>
-    <row r="37" spans="6:13" x14ac:dyDescent="0.3">
-      <c r="F37" s="43"/>
-      <c r="G37" s="47"/>
-      <c r="H37" s="45"/>
-      <c r="I37" s="45"/>
-      <c r="J37" s="45"/>
-      <c r="K37" s="45"/>
-      <c r="L37" s="45"/>
+    <row r="37" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F37" s="45"/>
+      <c r="G37" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="H37" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="I37" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="J37" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K37" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="L37" s="25"/>
       <c r="M37" s="46"/>
     </row>
-    <row r="38" spans="6:13" x14ac:dyDescent="0.3">
-      <c r="F38" s="43"/>
-      <c r="G38" s="51"/>
-      <c r="H38" s="52"/>
-      <c r="I38" s="45"/>
-      <c r="J38" s="45"/>
-      <c r="K38" s="45"/>
-      <c r="L38" s="50"/>
+    <row r="38" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F38" s="45"/>
+      <c r="G38" s="40">
+        <v>2047100</v>
+      </c>
+      <c r="H38" s="35">
+        <v>7.8499999999999994E-6</v>
+      </c>
+      <c r="I38" s="41">
+        <f>$A$19*H38</f>
+        <v>16.069734999999998</v>
+      </c>
+      <c r="J38" s="41">
+        <v>1.3852999999999999E-4</v>
+      </c>
+      <c r="K38" s="41">
+        <v>1.5971</v>
+      </c>
+      <c r="L38" s="39" t="s">
+        <v>11</v>
+      </c>
       <c r="M38" s="46"/>
     </row>
-    <row r="39" spans="6:13" x14ac:dyDescent="0.3">
-      <c r="F39" s="32"/>
-      <c r="G39" s="32"/>
-      <c r="H39" s="32"/>
-      <c r="I39" s="32"/>
-      <c r="J39" s="32"/>
-      <c r="K39" s="32"/>
-      <c r="L39" s="32"/>
-      <c r="M39" s="32"/>
-    </row>
-    <row r="40" spans="6:13" x14ac:dyDescent="0.3">
-      <c r="F40" s="32"/>
-      <c r="G40" s="32"/>
-      <c r="H40" s="32"/>
-      <c r="I40" s="32"/>
-      <c r="J40" s="32"/>
-      <c r="K40" s="32"/>
-      <c r="L40" s="32"/>
-      <c r="M40" s="32"/>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="F39" s="44"/>
+      <c r="G39" s="44"/>
+      <c r="H39" s="44"/>
+      <c r="I39" s="44"/>
+      <c r="J39" s="44"/>
+      <c r="K39" s="44"/>
+      <c r="L39" s="44"/>
+      <c r="M39" s="44"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="F40" s="44"/>
+      <c r="G40" s="44"/>
+      <c r="H40" s="44"/>
+      <c r="I40" s="44"/>
+      <c r="J40" s="44"/>
+      <c r="K40" s="44"/>
+      <c r="L40" s="44"/>
+      <c r="M40" s="44"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="14">
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="G5:L22"/>
@@ -1531,7 +1825,13 @@
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B22:C22"/>
+    <mergeCell ref="F24:M25"/>
     <mergeCell ref="F39:M40"/>
+    <mergeCell ref="F26:F33"/>
+    <mergeCell ref="M26:M33"/>
+    <mergeCell ref="F34:M35"/>
+    <mergeCell ref="F36:F38"/>
+    <mergeCell ref="M36:M38"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>